<commit_message>
Fixed storage calculation, Adjusted entities, Removed unnecessary attributes, Added js to enter to next focusfield, Added functions to display net weight and price, Re-worked front-end to suit commissioner request, Made Empty vendor selection in selectonemenu available by adding a string in case of null object.
</commit_message>
<xml_diff>
--- a/src/main/resources/form.xlsx
+++ b/src/main/resources/form.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Szilard\IdeaProjects\deliveryapplication\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Szilard\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{162B3AE9-5F44-4C6D-A154-7F9FCE58CD2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{76F9ADD5-9C21-4779-86D1-86753396040D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="11040" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1889,7 +1889,7 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,7 +1934,10 @@
       <c r="A6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="10">
+        <f ca="1">TODAY()</f>
+        <v>44988</v>
+      </c>
       <c r="C6" s="11"/>
       <c r="D6" s="12"/>
       <c r="E6" s="13"/>
@@ -2106,12 +2109,20 @@
       <c r="B25" s="34">
         <v>672</v>
       </c>
-      <c r="C25" s="34"/>
+      <c r="C25" s="34">
+        <v>0</v>
+      </c>
       <c r="D25" s="35">
         <v>0.05</v>
       </c>
-      <c r="E25" s="34"/>
-      <c r="F25" s="36"/>
+      <c r="E25" s="34">
+        <f>ROUNDDOWN(C25*0.95,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="36">
+        <f t="shared" ref="F25:F30" si="0">SUM(B25*E25)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
@@ -2120,12 +2131,20 @@
       <c r="B26" s="34">
         <v>560</v>
       </c>
-      <c r="C26" s="34"/>
+      <c r="C26" s="34">
+        <v>0</v>
+      </c>
       <c r="D26" s="35">
         <v>0.05</v>
       </c>
-      <c r="E26" s="34"/>
-      <c r="F26" s="36"/>
+      <c r="E26" s="34">
+        <f>ROUNDDOWN(C26*0.95,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
@@ -2134,12 +2153,20 @@
       <c r="B27" s="34">
         <v>448</v>
       </c>
-      <c r="C27" s="34"/>
+      <c r="C27" s="34">
+        <v>0</v>
+      </c>
       <c r="D27" s="35">
         <v>0.05</v>
       </c>
-      <c r="E27" s="34"/>
-      <c r="F27" s="36"/>
+      <c r="E27" s="34">
+        <f>ROUNDDOWN(C27*0.95,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
@@ -2148,12 +2175,19 @@
       <c r="B28" s="34">
         <v>224</v>
       </c>
-      <c r="C28" s="34"/>
+      <c r="C28" s="34">
+        <v>0</v>
+      </c>
       <c r="D28" s="35">
         <v>0.05</v>
       </c>
-      <c r="E28" s="34"/>
-      <c r="F28" s="36"/>
+      <c r="E28" s="34">
+        <v>0</v>
+      </c>
+      <c r="F28" s="36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
@@ -2162,12 +2196,19 @@
       <c r="B29" s="34">
         <v>56</v>
       </c>
-      <c r="C29" s="34"/>
+      <c r="C29" s="34">
+        <v>0</v>
+      </c>
       <c r="D29" s="35">
         <v>0.05</v>
       </c>
-      <c r="E29" s="34"/>
-      <c r="F29" s="36"/>
+      <c r="E29" s="34">
+        <v>0</v>
+      </c>
+      <c r="F29" s="36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="33" t="s">
@@ -2176,12 +2217,20 @@
       <c r="B30" s="34">
         <v>300</v>
       </c>
-      <c r="C30" s="34"/>
+      <c r="C30" s="34">
+        <v>0</v>
+      </c>
       <c r="D30" s="37">
         <v>0.08</v>
       </c>
-      <c r="E30" s="34"/>
-      <c r="F30" s="36"/>
+      <c r="E30" s="34">
+        <f>ROUNDDOWN(C30*0.95,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F30" s="36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="38" t="s">
@@ -2190,8 +2239,14 @@
       <c r="B31" s="39"/>
       <c r="C31" s="12"/>
       <c r="D31" s="13"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="41"/>
+      <c r="E31" s="40">
+        <f>SUM(E25:E30)</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="41">
+        <f>SUM(F25:F30)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="42"/>
@@ -2210,7 +2265,10 @@
         <v>38</v>
       </c>
       <c r="E33" s="40"/>
-      <c r="F33" s="48"/>
+      <c r="F33" s="48">
+        <f>SUM(F31-F32)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
@@ -2248,10 +2306,22 @@
         <v>40</v>
       </c>
       <c r="B40" s="45"/>
-      <c r="C40" s="50"/>
-      <c r="D40" s="50"/>
-      <c r="E40" s="51"/>
-      <c r="F40" s="52"/>
+      <c r="C40" s="50" t="e">
+        <f>ROUND(F40/1.12,0)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D40" s="50" t="e">
+        <f>SUM(F40-C40)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E40" s="51" t="e">
+        <f>ROUND(F31/E31,2)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F40" s="52" t="e">
+        <f>ROUND(E31*E40,0)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="41" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="49" t="s">
@@ -2260,7 +2330,10 @@
       <c r="B41" s="45"/>
       <c r="C41" s="53"/>
       <c r="D41" s="53"/>
-      <c r="E41" s="53"/>
+      <c r="E41" s="53" t="e">
+        <f>ROUND(E40/1.12,2)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="F41" s="29"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Reworked completed purchase frontend
</commit_message>
<xml_diff>
--- a/src/main/resources/form.xlsx
+++ b/src/main/resources/form.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Szilard\IdeaProjects\deliveryapplication\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\IdeaProjects\deliveryapplication\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09FB402-10F2-49B8-A653-9E9F2DB482B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E1AF8C-7017-45BA-A394-601DDD009E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49560" yWindow="12600" windowWidth="17640" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -126,9 +126,6 @@
     <t>ÖCSG SZÁM:</t>
   </si>
   <si>
-    <t>GGN SZÁM:</t>
-  </si>
-  <si>
     <t>TELEFONSZÁM:</t>
   </si>
   <si>
@@ -196,6 +193,9 @@
   </si>
   <si>
     <t>Töltse ki</t>
+  </si>
+  <si>
+    <t>NEBIH:</t>
   </si>
 </sst>
 </file>
@@ -627,7 +627,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -707,6 +707,9 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" pivotButton="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hivatkozás" xfId="2" builtinId="8"/>
@@ -1892,20 +1895,20 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1913,11 +1916,11 @@
       <c r="E1" s="2"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A3" s="6"/>
       <c r="C3" s="7" t="s">
         <v>0</v>
@@ -1925,21 +1928,21 @@
       <c r="D3" s="7"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="10">
         <f ca="1">TODAY()</f>
-        <v>45028</v>
+        <v>45118</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="12"/>
@@ -1948,22 +1951,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
       <c r="D7" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="16"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="59"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="D8" s="17" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="17"/>
-    </row>
-    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F8" s="59"/>
+    </row>
+    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="14"/>
       <c r="B9" s="15" t="s">
         <v>5</v>
@@ -1972,8 +1977,9 @@
         <v>6</v>
       </c>
       <c r="E9" s="19"/>
-    </row>
-    <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F9" s="59"/>
+    </row>
+    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="14"/>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
@@ -1981,8 +1987,9 @@
         <v>7</v>
       </c>
       <c r="E10" s="17"/>
-    </row>
-    <row r="11" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="F10" s="59"/>
+    </row>
+    <row r="11" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A11" s="20" t="s">
         <v>8</v>
       </c>
@@ -1992,15 +1999,17 @@
         <v>9</v>
       </c>
       <c r="E11" s="17"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="59"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="D12" s="17" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="17"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="59"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
@@ -2008,8 +2017,9 @@
         <v>12</v>
       </c>
       <c r="E13" s="19"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="59"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
@@ -2017,8 +2027,9 @@
         <v>14</v>
       </c>
       <c r="E14" s="17"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="59"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
@@ -2026,88 +2037,95 @@
         <v>16</v>
       </c>
       <c r="E15" s="17"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="59"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="D16" s="17" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="17"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="59"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="D17" s="18" t="s">
         <v>18</v>
       </c>
       <c r="E17" s="19"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="59"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="D18" s="17" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="E18" s="17"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="59"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="D19" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E19" s="17"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="59"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="D20" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E20" s="17"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="59"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
       <c r="B21" s="23"/>
       <c r="C21" s="24"/>
       <c r="D21" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E21" s="25"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F21" s="59"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="26"/>
       <c r="B23" s="27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" s="28"/>
       <c r="D23" s="28"/>
       <c r="E23" s="28"/>
       <c r="F23" s="29"/>
     </row>
-    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="C24" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="D24" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="31" t="s">
+      <c r="E24" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="31" t="s">
+      <c r="F24" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="32" t="s">
+    </row>
+    <row r="25" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="33" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
-        <v>30</v>
       </c>
       <c r="B25" s="34">
         <v>672</v>
@@ -2127,9 +2145,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" s="34">
         <v>560</v>
@@ -2149,9 +2167,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" s="34">
         <v>448</v>
@@ -2171,9 +2189,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" s="34">
         <v>224</v>
@@ -2192,9 +2210,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29" s="34">
         <v>56</v>
@@ -2213,9 +2231,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" s="34">
         <v>300</v>
@@ -2235,9 +2253,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" s="38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" s="39"/>
       <c r="C31" s="12"/>
@@ -2251,23 +2269,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="42"/>
       <c r="B32" s="43"/>
       <c r="C32" s="44"/>
       <c r="D32" s="45" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E32" s="45"/>
       <c r="F32" s="36" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A33" s="4"/>
       <c r="C33" s="46"/>
       <c r="D33" s="47" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E33" s="40"/>
       <c r="F33" s="48">
@@ -2275,26 +2293,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="F35" s="5"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4"/>
       <c r="F37" s="5"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -2302,13 +2320,13 @@
       <c r="E38" s="2"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="F39" s="5"/>
     </row>
-    <row r="40" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A40" s="49" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40" s="45"/>
       <c r="C40" s="50" t="e">
@@ -2328,9 +2346,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A41" s="49" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" s="45"/>
       <c r="C41" s="53"/>
@@ -2341,11 +2359,11 @@
       </c>
       <c r="F41" s="29"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="F42" s="5"/>
     </row>
-    <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="54"/>
       <c r="B43" s="55"/>
       <c r="C43" s="56"/>
@@ -2355,5 +2373,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Form adjusted for Excel type download; Modified commandButtons to dismiss concerns about Mojara's potential errors and repair functionality to completedpurchase_content.xhtml
</commit_message>
<xml_diff>
--- a/src/main/resources/form.xlsx
+++ b/src/main/resources/form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\IdeaProjects\deliveryapplication\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E1AF8C-7017-45BA-A394-601DDD009E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040A8FD2-6E18-453D-BEAF-7DED3C0BB82E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -314,7 +314,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -616,6 +616,30 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -627,7 +651,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -707,7 +731,10 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" pivotButton="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -716,7 +743,35 @@
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
     <cellStyle name="Százalék" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="22">
+    <dxf>
+      <border>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thick">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thick">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <right style="medium">
@@ -1361,21 +1416,21 @@
     <field x="13"/>
     <field x="14"/>
   </rowFields>
-  <formats count="18">
-    <format dxfId="17">
+  <formats count="20">
+    <format dxfId="21">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="16">
+    <format dxfId="20">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="15">
+    <format dxfId="19">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0" selected="0"/>
@@ -1383,7 +1438,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="17">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="0" selected="0"/>
@@ -1392,7 +1447,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="16">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="4">
           <reference field="0" count="0" selected="0"/>
@@ -1402,7 +1457,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="11">
+    <format dxfId="15">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="5">
           <reference field="0" count="0" selected="0"/>
@@ -1413,7 +1468,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="6">
           <reference field="0" count="0" selected="0"/>
@@ -1425,7 +1480,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="7">
           <reference field="0" count="0" selected="0"/>
@@ -1438,7 +1493,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="8">
           <reference field="0" count="0" selected="0"/>
@@ -1452,7 +1507,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="11">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="9">
           <reference field="0" count="0" selected="0"/>
@@ -1467,7 +1522,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
+    <format dxfId="10">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="10">
           <reference field="0" count="0" selected="0"/>
@@ -1483,7 +1538,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="5">
+    <format dxfId="9">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="11">
           <reference field="0" count="0" selected="0"/>
@@ -1500,7 +1555,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="12">
           <reference field="0" count="0" selected="0"/>
@@ -1518,7 +1573,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="7">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="13">
           <reference field="0" count="0" selected="0"/>
@@ -1537,7 +1592,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="14">
           <reference field="0" count="0" selected="0"/>
@@ -1557,7 +1612,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="5">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="4">
+      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="3">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
     <format dxfId="0">
@@ -1894,8 +1955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1942,7 +2003,7 @@
       </c>
       <c r="B6" s="10">
         <f ca="1">TODAY()</f>
-        <v>45118</v>
+        <v>45132</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="12"/>
@@ -1966,7 +2027,7 @@
         <v>4</v>
       </c>
       <c r="E8" s="17"/>
-      <c r="F8" s="59"/>
+      <c r="F8" s="60"/>
     </row>
     <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="14"/>
@@ -1977,7 +2038,7 @@
         <v>6</v>
       </c>
       <c r="E9" s="19"/>
-      <c r="F9" s="59"/>
+      <c r="F9" s="60"/>
     </row>
     <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="14"/>
@@ -1987,7 +2048,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="17"/>
-      <c r="F10" s="59"/>
+      <c r="F10" s="60"/>
     </row>
     <row r="11" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A11" s="20" t="s">
@@ -1999,7 +2060,7 @@
         <v>9</v>
       </c>
       <c r="E11" s="17"/>
-      <c r="F11" s="59"/>
+      <c r="F11" s="60"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
@@ -2007,7 +2068,7 @@
         <v>10</v>
       </c>
       <c r="E12" s="17"/>
-      <c r="F12" s="59"/>
+      <c r="F12" s="60"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
@@ -2017,7 +2078,7 @@
         <v>12</v>
       </c>
       <c r="E13" s="19"/>
-      <c r="F13" s="59"/>
+      <c r="F13" s="60"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
@@ -2027,7 +2088,7 @@
         <v>14</v>
       </c>
       <c r="E14" s="17"/>
-      <c r="F14" s="59"/>
+      <c r="F14" s="60"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
@@ -2037,7 +2098,7 @@
         <v>16</v>
       </c>
       <c r="E15" s="17"/>
-      <c r="F15" s="59"/>
+      <c r="F15" s="60"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
@@ -2045,7 +2106,7 @@
         <v>17</v>
       </c>
       <c r="E16" s="17"/>
-      <c r="F16" s="59"/>
+      <c r="F16" s="60"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
@@ -2053,7 +2114,7 @@
         <v>18</v>
       </c>
       <c r="E17" s="19"/>
-      <c r="F17" s="59"/>
+      <c r="F17" s="60"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
@@ -2061,7 +2122,7 @@
         <v>42</v>
       </c>
       <c r="E18" s="17"/>
-      <c r="F18" s="59"/>
+      <c r="F18" s="60"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
@@ -2069,7 +2130,7 @@
         <v>19</v>
       </c>
       <c r="E19" s="17"/>
-      <c r="F19" s="59"/>
+      <c r="F19" s="60"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
@@ -2077,7 +2138,7 @@
         <v>20</v>
       </c>
       <c r="E20" s="17"/>
-      <c r="F20" s="59"/>
+      <c r="F20" s="60"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
@@ -2087,11 +2148,11 @@
         <v>21</v>
       </c>
       <c r="E21" s="25"/>
-      <c r="F21" s="59"/>
+      <c r="F21" s="60"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
-      <c r="F22" s="5"/>
+      <c r="F22" s="8"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="26"/>

</xml_diff>